<commit_message>
FIX: Match present values in episode 3
</commit_message>
<xml_diff>
--- a/PresentValueSeries/reproduce.xlsx
+++ b/PresentValueSeries/reproduce.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{282573E7-0B41-4DF6-ACDF-990296F9B510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B58AEC9-C7D7-4FB4-A7BE-5CEB1F90ABD2}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{282573E7-0B41-4DF6-ACDF-990296F9B510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C72D92C-193B-4251-80C3-AD7F868B54F2}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="3680" windowWidth="26380" windowHeight="13010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="4070" windowWidth="26380" windowHeight="13010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <definedName name="VariableType_DisplayName">#REF!</definedName>
     <definedName name="VariableType_SystemName">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcCompleted="0" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1362,6 +1362,9 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="YieldCurve"/>
       <sheetName val="ignore_SystemSheet"/>
@@ -1383,6 +1386,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1848,7 +1855,7 @@
   <dimension ref="A1:BU23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G5"/>
+      <selection activeCell="L15" sqref="L14:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1857,7 +1864,8 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4140625" customWidth="1"/>
+    <col min="6" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="25" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5676,7 +5684,7 @@
         <v>88</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:AJ21" ca="1" si="7">E7+F21*E$13</f>
+        <f t="shared" ref="E21:I21" ca="1" si="7">E7+F21*E$13</f>
         <v>18179.867502742232</v>
       </c>
       <c r="F21">

</xml_diff>